<commit_message>
Implemented live search, added inspector field and other changes.
1. Implemented live search in Dashboard page.
2. Added "inspector" data field to inspection certificates and made all necessary changes everywhere.
3. Removed unnecessary migration files and incorporated them in appropriate migration files. Also made necessary modifications for training certificate table.
4. Fixed Add New Certificate bug in View Certificate page.
5. Added contact info to Verify Certificate page.
</commit_message>
<xml_diff>
--- a/downloads/Inspection Data Import Template.xlsx
+++ b/downloads/Inspection Data Import Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\verify-cert-inspection\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71F1990-A971-4E34-8248-863078A2B9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F34BCB-C320-46E6-8F59-EDEBB81DB917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6375" yWindow="-30" windowWidth="22545" windowHeight="14835" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>certificate_number</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>inspection_internal_notes</t>
+  </si>
+  <si>
+    <t>inspector</t>
   </si>
 </sst>
 </file>
@@ -420,70 +423,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="2"/>
-    <col min="9" max="9" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="2" max="2" width="18.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="2"/>
+    <col min="10" max="10" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>